<commit_message>
Updated to include Very Heavy Trucks and other minor changes
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SubRES_TMPL/SubRES_NewTech_RC.xlsx
+++ b/TIMES-NZ/SubRES_TMPL/SubRES_NewTech_RC.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishwarc\Documents\2018 Electricity Generation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VEDA_Models\NZ_TIMES_model-v82\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB098A20-6F2F-4F9F-9EE8-AC4AFF5ECA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OTH_COM" sheetId="9" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OTH_COM!$C$3:$X$281</definedName>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2079,7 +2081,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2281,7 +2283,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2391,19 +2393,22 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 5" xfId="6"/>
-    <cellStyle name="Normal 29" xfId="4"/>
-    <cellStyle name="Normal 29 2" xfId="9"/>
-    <cellStyle name="Normal 30" xfId="7"/>
-    <cellStyle name="Normal 30 2" xfId="8"/>
-    <cellStyle name="Normal 30 2 2" xfId="11"/>
-    <cellStyle name="Normal 30 3" xfId="10"/>
-    <cellStyle name="Normal 4 10" xfId="5"/>
-    <cellStyle name="Normale_B2020" xfId="2"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 10 5" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 29" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 29 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 30" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 30 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 30 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 30 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4 10" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normale_B2020" xfId="2" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2630,6 +2635,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2665,6 +2687,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2840,15 +2879,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="C3:X1204"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="G3" sqref="G3"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
-      <selection pane="bottomRight" activeCell="AB23" sqref="AB23"/>
+      <selection pane="bottomRight" activeCell="V253" sqref="V253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,7 +2914,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="3:24" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:24" ht="22.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2942,7 +2982,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="5" spans="3:24" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:24" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
@@ -2986,7 +3026,7 @@
       <c r="W5" s="11"/>
       <c r="X5" s="9"/>
     </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C6" s="12" t="s">
         <v>48</v>
       </c>
@@ -3027,13 +3067,13 @@
       <c r="T6" s="16">
         <v>0</v>
       </c>
-      <c r="U6" s="16">
+      <c r="U6" s="67">
         <v>0.216895</v>
       </c>
       <c r="V6" s="61"/>
       <c r="W6" s="61"/>
     </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>52</v>
       </c>
@@ -3070,14 +3110,14 @@
       <c r="T7" s="16">
         <v>0</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="67">
         <v>0.216895</v>
       </c>
       <c r="V7" s="65"/>
       <c r="W7" s="65"/>
       <c r="X7" s="66"/>
     </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C8" s="12" t="s">
         <v>55</v>
       </c>
@@ -3114,14 +3154,14 @@
       <c r="T8" s="16">
         <v>0</v>
       </c>
-      <c r="U8" s="16">
+      <c r="U8" s="67">
         <v>0.216895</v>
       </c>
       <c r="V8" s="65"/>
       <c r="W8" s="65"/>
       <c r="X8" s="66"/>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
         <v>57</v>
       </c>
@@ -3162,13 +3202,13 @@
       <c r="T9" s="16">
         <v>0</v>
       </c>
-      <c r="U9" s="16">
+      <c r="U9" s="67">
         <v>0.216895</v>
       </c>
       <c r="V9" s="61"/>
       <c r="W9" s="61"/>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C10" s="12" t="s">
         <v>59</v>
       </c>
@@ -3205,8 +3245,8 @@
       <c r="T10" s="16">
         <v>15</v>
       </c>
-      <c r="U10" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U10" s="67">
+        <v>0.1</v>
       </c>
       <c r="V10" s="61">
         <v>0.05</v>
@@ -3218,7 +3258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C11" s="12" t="s">
         <v>63</v>
       </c>
@@ -3255,8 +3295,8 @@
       <c r="T11" s="16">
         <v>3</v>
       </c>
-      <c r="U11" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U11" s="67">
+        <v>0.1</v>
       </c>
       <c r="V11" s="61">
         <v>0.01</v>
@@ -3268,7 +3308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="12" t="s">
         <v>66</v>
       </c>
@@ -3305,8 +3345,8 @@
       <c r="T12" s="16">
         <v>3</v>
       </c>
-      <c r="U12" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U12" s="67">
+        <v>0.1</v>
       </c>
       <c r="V12" s="61">
         <v>0</v>
@@ -3318,7 +3358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C13" s="12" t="s">
         <v>69</v>
       </c>
@@ -3355,8 +3395,8 @@
       <c r="T13" s="16">
         <v>2</v>
       </c>
-      <c r="U13" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U13" s="67">
+        <v>0.1</v>
       </c>
       <c r="V13" s="63">
         <v>0</v>
@@ -3368,7 +3408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C14" s="12" t="s">
         <v>72</v>
       </c>
@@ -3405,8 +3445,8 @@
       <c r="T14" s="16">
         <v>2</v>
       </c>
-      <c r="U14" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U14" s="67">
+        <v>0.1</v>
       </c>
       <c r="V14" s="61">
         <v>0.19550000000000001</v>
@@ -3418,7 +3458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="12" t="s">
         <v>75</v>
       </c>
@@ -3455,8 +3495,8 @@
       <c r="T15" s="16">
         <v>10</v>
       </c>
-      <c r="U15" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U15" s="67">
+        <v>0.1</v>
       </c>
       <c r="V15" s="61">
         <v>0.2</v>
@@ -3468,7 +3508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
         <v>78</v>
       </c>
@@ -3505,8 +3545,8 @@
       <c r="T16" s="16">
         <v>10</v>
       </c>
-      <c r="U16" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U16" s="67">
+        <v>0.1</v>
       </c>
       <c r="V16" s="61">
         <v>0.2</v>
@@ -3518,7 +3558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C17" s="12" t="s">
         <v>81</v>
       </c>
@@ -3555,8 +3595,8 @@
       <c r="T17" s="16">
         <v>2</v>
       </c>
-      <c r="U17" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U17" s="67">
+        <v>0.1</v>
       </c>
       <c r="V17" s="61">
         <v>0.1</v>
@@ -3568,7 +3608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C18" s="12" t="s">
         <v>83</v>
       </c>
@@ -3605,8 +3645,8 @@
       <c r="T18" s="16">
         <v>2</v>
       </c>
-      <c r="U18" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U18" s="67">
+        <v>0.1</v>
       </c>
       <c r="V18" s="61">
         <v>0</v>
@@ -3655,8 +3695,8 @@
       <c r="T19" s="16">
         <v>2</v>
       </c>
-      <c r="U19" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U19" s="67">
+        <v>0.1</v>
       </c>
       <c r="V19" s="61">
         <v>0</v>
@@ -3668,7 +3708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C20" s="12" t="s">
         <v>89</v>
       </c>
@@ -3705,7 +3745,7 @@
       <c r="T20" s="16">
         <v>15</v>
       </c>
-      <c r="U20" s="16">
+      <c r="U20" s="67">
         <v>0.216895</v>
       </c>
       <c r="V20" s="61">
@@ -3718,7 +3758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="12" t="s">
         <v>91</v>
       </c>
@@ -3755,7 +3795,7 @@
       <c r="T21" s="16">
         <v>3</v>
       </c>
-      <c r="U21" s="16">
+      <c r="U21" s="67">
         <v>0.216895</v>
       </c>
       <c r="V21" s="61">
@@ -3768,7 +3808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C22" s="12" t="s">
         <v>92</v>
       </c>
@@ -3805,7 +3845,7 @@
       <c r="T22" s="16">
         <v>3</v>
       </c>
-      <c r="U22" s="16">
+      <c r="U22" s="67">
         <v>0.216895</v>
       </c>
       <c r="V22" s="61">
@@ -3818,7 +3858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C23" s="12" t="s">
         <v>93</v>
       </c>
@@ -3855,7 +3895,7 @@
       <c r="T23" s="16">
         <v>2</v>
       </c>
-      <c r="U23" s="16">
+      <c r="U23" s="67">
         <v>0.216895</v>
       </c>
       <c r="V23" s="61">
@@ -3868,7 +3908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C24" s="12" t="s">
         <v>94</v>
       </c>
@@ -3905,7 +3945,7 @@
       <c r="T24" s="16">
         <v>2</v>
       </c>
-      <c r="U24" s="16">
+      <c r="U24" s="67">
         <v>0.216895</v>
       </c>
       <c r="V24" s="61">
@@ -3918,7 +3958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C25" s="12" t="s">
         <v>95</v>
       </c>
@@ -3955,13 +3995,13 @@
       <c r="T25" s="16">
         <v>10</v>
       </c>
-      <c r="U25" s="16">
+      <c r="U25" s="67">
         <v>0.216895</v>
       </c>
       <c r="V25" s="61"/>
       <c r="W25" s="61"/>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" s="12" t="s">
         <v>96</v>
       </c>
@@ -3998,13 +4038,13 @@
       <c r="T26" s="16">
         <v>10</v>
       </c>
-      <c r="U26" s="16">
+      <c r="U26" s="67">
         <v>0.216895</v>
       </c>
       <c r="V26" s="61"/>
       <c r="W26" s="61"/>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>97</v>
       </c>
@@ -4041,7 +4081,7 @@
       <c r="T27" s="16">
         <v>2</v>
       </c>
-      <c r="U27" s="16">
+      <c r="U27" s="67">
         <v>0.216895</v>
       </c>
       <c r="V27" s="61">
@@ -4054,7 +4094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C28" s="12" t="s">
         <v>98</v>
       </c>
@@ -4091,7 +4131,7 @@
       <c r="T28" s="16">
         <v>2</v>
       </c>
-      <c r="U28" s="16">
+      <c r="U28" s="67">
         <v>0.216895</v>
       </c>
       <c r="V28" s="61">
@@ -4141,7 +4181,7 @@
       <c r="T29" s="16">
         <v>2</v>
       </c>
-      <c r="U29" s="16">
+      <c r="U29" s="67">
         <v>0.216895</v>
       </c>
       <c r="V29" s="61">
@@ -4154,7 +4194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="3:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="12" t="s">
         <v>100</v>
       </c>
@@ -4201,8 +4241,8 @@
       <c r="T30" s="16">
         <v>0</v>
       </c>
-      <c r="U30" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U30" s="67">
+        <v>0.1</v>
       </c>
       <c r="V30" s="62">
         <v>0.3</v>
@@ -4214,7 +4254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C31" s="12" t="s">
         <v>149</v>
       </c>
@@ -4245,11 +4285,11 @@
       <c r="R31" s="16"/>
       <c r="S31" s="16"/>
       <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
+      <c r="U31" s="67"/>
       <c r="V31" s="62"/>
       <c r="W31" s="62"/>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>103</v>
       </c>
@@ -4296,8 +4336,8 @@
       <c r="T32" s="16">
         <v>0</v>
       </c>
-      <c r="U32" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U32" s="67">
+        <v>0.1</v>
       </c>
       <c r="V32" s="61">
         <v>0.3</v>
@@ -4309,7 +4349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C33" s="12" t="s">
         <v>149</v>
       </c>
@@ -4340,11 +4380,11 @@
       <c r="R33" s="16"/>
       <c r="S33" s="16"/>
       <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
+      <c r="U33" s="67"/>
       <c r="V33" s="61"/>
       <c r="W33" s="61"/>
     </row>
-    <row r="34" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C34" s="12" t="s">
         <v>105</v>
       </c>
@@ -4381,8 +4421,8 @@
       <c r="T34" s="16">
         <v>0</v>
       </c>
-      <c r="U34" s="16">
-        <v>0.16267100000000001</v>
+      <c r="U34" s="67">
+        <v>0.1</v>
       </c>
       <c r="V34" s="61">
         <v>0.5</v>
@@ -4394,7 +4434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C35" s="12" t="s">
         <v>107</v>
       </c>
@@ -4439,7 +4479,7 @@
       <c r="T35" s="16">
         <v>0</v>
       </c>
-      <c r="U35" s="16">
+      <c r="U35" s="67">
         <v>0.216895</v>
       </c>
       <c r="V35" s="61">
@@ -4452,7 +4492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C36" s="12" t="s">
         <v>108</v>
       </c>
@@ -4497,7 +4537,7 @@
       <c r="T36" s="16">
         <v>0</v>
       </c>
-      <c r="U36" s="16">
+      <c r="U36" s="67">
         <v>0.216895</v>
       </c>
       <c r="V36" s="61">
@@ -4510,7 +4550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C37" s="12" t="s">
         <v>109</v>
       </c>
@@ -4547,7 +4587,7 @@
       <c r="T37" s="16">
         <v>0</v>
       </c>
-      <c r="U37" s="16">
+      <c r="U37" s="67">
         <v>0.216895</v>
       </c>
       <c r="V37" s="61">
@@ -4560,7 +4600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C38" s="12" t="s">
         <v>111</v>
       </c>
@@ -4597,7 +4637,7 @@
       <c r="T38" s="16">
         <v>0</v>
       </c>
-      <c r="U38" s="16">
+      <c r="U38" s="67">
         <v>0.216895</v>
       </c>
       <c r="V38" s="61">
@@ -4610,7 +4650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C39" s="12" t="s">
         <v>113</v>
       </c>
@@ -4647,7 +4687,7 @@
       <c r="T39" s="16">
         <v>0</v>
       </c>
-      <c r="U39" s="16">
+      <c r="U39" s="67">
         <v>0.216895</v>
       </c>
       <c r="V39" s="61">
@@ -4660,7 +4700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C40" s="12" t="s">
         <v>115</v>
       </c>
@@ -4697,7 +4737,7 @@
       <c r="T40" s="16">
         <v>0</v>
       </c>
-      <c r="U40" s="16">
+      <c r="U40" s="67">
         <v>0.216895</v>
       </c>
       <c r="V40" s="61">
@@ -4710,7 +4750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C41" s="12" t="s">
         <v>117</v>
       </c>
@@ -4747,7 +4787,7 @@
       <c r="T41" s="16">
         <v>0</v>
       </c>
-      <c r="U41" s="16">
+      <c r="U41" s="67">
         <v>0.216895</v>
       </c>
       <c r="V41" s="61">
@@ -4760,7 +4800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C42" s="12" t="s">
         <v>119</v>
       </c>
@@ -4797,7 +4837,7 @@
       <c r="T42" s="16">
         <v>0</v>
       </c>
-      <c r="U42" s="16">
+      <c r="U42" s="67">
         <v>0.216895</v>
       </c>
       <c r="V42" s="61">
@@ -4810,7 +4850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C43" s="12" t="s">
         <v>121</v>
       </c>
@@ -4847,7 +4887,7 @@
       <c r="T43" s="16">
         <v>7</v>
       </c>
-      <c r="U43" s="16">
+      <c r="U43" s="67">
         <v>0.05</v>
       </c>
       <c r="V43" s="61">
@@ -4860,7 +4900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C44" s="12" t="s">
         <v>124</v>
       </c>
@@ -4897,7 +4937,7 @@
       <c r="T44" s="16">
         <v>7</v>
       </c>
-      <c r="U44" s="16">
+      <c r="U44" s="67">
         <v>0.05</v>
       </c>
       <c r="V44" s="61">
@@ -4910,7 +4950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C45" s="12" t="s">
         <v>127</v>
       </c>
@@ -4947,13 +4987,13 @@
       <c r="T45" s="16">
         <v>7</v>
       </c>
-      <c r="U45" s="16">
+      <c r="U45" s="67">
         <v>0.05</v>
       </c>
       <c r="V45" s="61"/>
       <c r="W45" s="61"/>
     </row>
-    <row r="46" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" s="12" t="s">
         <v>129</v>
       </c>
@@ -4990,7 +5030,7 @@
       <c r="T46" s="16">
         <v>0</v>
       </c>
-      <c r="U46" s="16">
+      <c r="U46" s="67">
         <v>0.05</v>
       </c>
       <c r="V46" s="61">
@@ -5048,7 +5088,7 @@
       <c r="T47" s="16">
         <v>2</v>
       </c>
-      <c r="U47" s="16">
+      <c r="U47" s="67">
         <v>0.05</v>
       </c>
       <c r="V47" s="61">
@@ -5061,7 +5101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C48" s="12" t="s">
         <v>133</v>
       </c>
@@ -5098,7 +5138,7 @@
       <c r="T48" s="16">
         <v>5</v>
       </c>
-      <c r="U48" s="16">
+      <c r="U48" s="67">
         <v>0.216895</v>
       </c>
       <c r="V48" s="61">
@@ -5111,7 +5151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C49" s="12" t="s">
         <v>136</v>
       </c>
@@ -5148,7 +5188,7 @@
       <c r="T49" s="16">
         <v>5</v>
       </c>
-      <c r="U49" s="16">
+      <c r="U49" s="67">
         <v>0.216895</v>
       </c>
       <c r="V49" s="61">
@@ -5161,7 +5201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C50" s="12" t="s">
         <v>138</v>
       </c>
@@ -5198,13 +5238,13 @@
       <c r="T50" s="16">
         <v>5</v>
       </c>
-      <c r="U50" s="16">
+      <c r="U50" s="67">
         <v>0.216895</v>
       </c>
       <c r="V50" s="61"/>
       <c r="W50" s="61"/>
     </row>
-    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C51" s="12" t="s">
         <v>140</v>
       </c>
@@ -5245,7 +5285,7 @@
       <c r="T51" s="16">
         <v>0</v>
       </c>
-      <c r="U51" s="16">
+      <c r="U51" s="67">
         <v>0.216895</v>
       </c>
       <c r="V51" s="61">
@@ -5303,7 +5343,7 @@
       <c r="T52" s="16">
         <v>2</v>
       </c>
-      <c r="U52" s="16">
+      <c r="U52" s="67">
         <v>0.216895</v>
       </c>
       <c r="V52" s="61">
@@ -5316,7 +5356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C53" s="12" t="s">
         <v>144</v>
       </c>
@@ -5353,13 +5393,13 @@
       <c r="T53" s="16">
         <v>5</v>
       </c>
-      <c r="U53" s="16">
+      <c r="U53" s="67">
         <v>0.216895</v>
       </c>
       <c r="V53" s="61"/>
       <c r="W53" s="61"/>
     </row>
-    <row r="54" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C54" s="12" t="s">
         <v>548</v>
       </c>
@@ -5404,13 +5444,13 @@
       <c r="T54" s="16">
         <v>0</v>
       </c>
-      <c r="U54" s="16">
+      <c r="U54" s="67">
         <v>0.108447</v>
       </c>
       <c r="V54" s="61"/>
       <c r="W54" s="61"/>
     </row>
-    <row r="55" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C55" s="12" t="s">
         <v>549</v>
       </c>
@@ -5455,13 +5495,13 @@
       <c r="T55" s="16">
         <v>0</v>
       </c>
-      <c r="U55" s="16">
+      <c r="U55" s="67">
         <v>0.108447</v>
       </c>
       <c r="V55" s="61"/>
       <c r="W55" s="61"/>
     </row>
-    <row r="56" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C56" s="12" t="s">
         <v>149</v>
       </c>
@@ -5486,11 +5526,11 @@
       <c r="R56" s="16"/>
       <c r="S56" s="16"/>
       <c r="T56" s="16"/>
-      <c r="U56" s="16"/>
+      <c r="U56" s="67"/>
       <c r="V56" s="61"/>
       <c r="W56" s="61"/>
     </row>
-    <row r="57" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C57" s="12" t="s">
         <v>150</v>
       </c>
@@ -5531,13 +5571,13 @@
       <c r="T57" s="16">
         <v>0</v>
       </c>
-      <c r="U57" s="16">
+      <c r="U57" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V57" s="61"/>
       <c r="W57" s="61"/>
     </row>
-    <row r="58" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C58" s="12" t="s">
         <v>153</v>
       </c>
@@ -5574,13 +5614,13 @@
       <c r="T58" s="16">
         <v>0</v>
       </c>
-      <c r="U58" s="16">
+      <c r="U58" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V58" s="65"/>
       <c r="W58" s="61"/>
     </row>
-    <row r="59" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C59" s="12" t="s">
         <v>156</v>
       </c>
@@ -5617,13 +5657,13 @@
       <c r="T59" s="16">
         <v>0</v>
       </c>
-      <c r="U59" s="16">
+      <c r="U59" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V59" s="65"/>
       <c r="W59" s="61"/>
     </row>
-    <row r="60" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C60" s="12" t="s">
         <v>158</v>
       </c>
@@ -5664,13 +5704,13 @@
       <c r="T60" s="16">
         <v>0</v>
       </c>
-      <c r="U60" s="16">
+      <c r="U60" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V60" s="61"/>
       <c r="W60" s="61"/>
     </row>
-    <row r="61" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C61" s="12" t="s">
         <v>160</v>
       </c>
@@ -5707,7 +5747,7 @@
       <c r="T61" s="16">
         <v>15</v>
       </c>
-      <c r="U61" s="16">
+      <c r="U61" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V61" s="61">
@@ -5720,7 +5760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" s="12" t="s">
         <v>163</v>
       </c>
@@ -5757,7 +5797,7 @@
       <c r="T62" s="16">
         <v>3</v>
       </c>
-      <c r="U62" s="16">
+      <c r="U62" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V62" s="61">
@@ -5770,7 +5810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C63" s="12" t="s">
         <v>165</v>
       </c>
@@ -5807,7 +5847,7 @@
       <c r="T63" s="16">
         <v>3</v>
       </c>
-      <c r="U63" s="16">
+      <c r="U63" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V63" s="61">
@@ -5820,7 +5860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C64" s="12" t="s">
         <v>167</v>
       </c>
@@ -5857,7 +5897,7 @@
       <c r="T64" s="16">
         <v>2</v>
       </c>
-      <c r="U64" s="16">
+      <c r="U64" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V64" s="61">
@@ -5870,7 +5910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C65" s="12" t="s">
         <v>169</v>
       </c>
@@ -5907,7 +5947,7 @@
       <c r="T65" s="16">
         <v>2</v>
       </c>
-      <c r="U65" s="16">
+      <c r="U65" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V65" s="61">
@@ -5920,7 +5960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C66" s="12" t="s">
         <v>171</v>
       </c>
@@ -5957,7 +5997,7 @@
       <c r="T66" s="16">
         <v>10</v>
       </c>
-      <c r="U66" s="16">
+      <c r="U66" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V66" s="61">
@@ -5970,7 +6010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C67" s="12" t="s">
         <v>173</v>
       </c>
@@ -6007,7 +6047,7 @@
       <c r="T67" s="16">
         <v>10</v>
       </c>
-      <c r="U67" s="16">
+      <c r="U67" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V67" s="61">
@@ -6020,7 +6060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" s="12" t="s">
         <v>175</v>
       </c>
@@ -6057,7 +6097,7 @@
       <c r="T68" s="16">
         <v>2</v>
       </c>
-      <c r="U68" s="16">
+      <c r="U68" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V68" s="61">
@@ -6070,7 +6110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C69" s="12" t="s">
         <v>177</v>
       </c>
@@ -6107,7 +6147,7 @@
       <c r="T69" s="16">
         <v>2</v>
       </c>
-      <c r="U69" s="16">
+      <c r="U69" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V69" s="61">
@@ -6157,20 +6197,20 @@
       <c r="T70" s="16">
         <v>2</v>
       </c>
-      <c r="U70" s="16">
+      <c r="U70" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V70" s="61">
         <v>0</v>
       </c>
       <c r="W70" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X70" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" s="12" t="s">
         <v>181</v>
       </c>
@@ -6207,7 +6247,7 @@
       <c r="T71" s="16">
         <v>15</v>
       </c>
-      <c r="U71" s="16">
+      <c r="U71" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V71" s="61">
@@ -6220,7 +6260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="3:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="12" t="s">
         <v>183</v>
       </c>
@@ -6257,7 +6297,7 @@
       <c r="T72" s="16">
         <v>3</v>
       </c>
-      <c r="U72" s="16">
+      <c r="U72" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V72" s="61">
@@ -6270,7 +6310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C73" s="12" t="s">
         <v>184</v>
       </c>
@@ -6307,7 +6347,7 @@
       <c r="T73" s="16">
         <v>3</v>
       </c>
-      <c r="U73" s="16">
+      <c r="U73" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V73" s="61">
@@ -6320,7 +6360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74" s="12" t="s">
         <v>185</v>
       </c>
@@ -6357,7 +6397,7 @@
       <c r="T74" s="16">
         <v>2</v>
       </c>
-      <c r="U74" s="16">
+      <c r="U74" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V74" s="61">
@@ -6370,7 +6410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C75" s="12" t="s">
         <v>186</v>
       </c>
@@ -6407,7 +6447,7 @@
       <c r="T75" s="16">
         <v>2</v>
       </c>
-      <c r="U75" s="16">
+      <c r="U75" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V75" s="61">
@@ -6420,7 +6460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="12" t="s">
         <v>187</v>
       </c>
@@ -6457,7 +6497,7 @@
       <c r="T76" s="16">
         <v>10</v>
       </c>
-      <c r="U76" s="16">
+      <c r="U76" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V76" s="61">
@@ -6470,7 +6510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C77" s="12" t="s">
         <v>188</v>
       </c>
@@ -6507,7 +6547,7 @@
       <c r="T77" s="16">
         <v>10</v>
       </c>
-      <c r="U77" s="16">
+      <c r="U77" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V77" s="61">
@@ -6520,7 +6560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C78" s="12" t="s">
         <v>189</v>
       </c>
@@ -6557,7 +6597,7 @@
       <c r="T78" s="16">
         <v>2</v>
       </c>
-      <c r="U78" s="16">
+      <c r="U78" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V78" s="61">
@@ -6570,7 +6610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C79" s="12" t="s">
         <v>190</v>
       </c>
@@ -6607,7 +6647,7 @@
       <c r="T79" s="16">
         <v>2</v>
       </c>
-      <c r="U79" s="16">
+      <c r="U79" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V79" s="61">
@@ -6657,20 +6697,20 @@
       <c r="T80" s="16">
         <v>2</v>
       </c>
-      <c r="U80" s="16">
+      <c r="U80" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V80" s="61">
         <v>0</v>
       </c>
       <c r="W80" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X80" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C81" s="12" t="s">
         <v>192</v>
       </c>
@@ -6707,7 +6747,7 @@
       <c r="T81" s="16">
         <v>15</v>
       </c>
-      <c r="U81" s="16">
+      <c r="U81" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V81" s="61">
@@ -6720,7 +6760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C82" s="12" t="s">
         <v>194</v>
       </c>
@@ -6757,7 +6797,7 @@
       <c r="T82" s="16">
         <v>3</v>
       </c>
-      <c r="U82" s="16">
+      <c r="U82" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V82" s="61">
@@ -6770,7 +6810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C83" s="12" t="s">
         <v>195</v>
       </c>
@@ -6807,7 +6847,7 @@
       <c r="T83" s="16">
         <v>3</v>
       </c>
-      <c r="U83" s="16">
+      <c r="U83" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V83" s="61">
@@ -6820,7 +6860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C84" s="12" t="s">
         <v>196</v>
       </c>
@@ -6857,7 +6897,7 @@
       <c r="T84" s="16">
         <v>2</v>
       </c>
-      <c r="U84" s="16">
+      <c r="U84" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V84" s="61">
@@ -6870,7 +6910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C85" s="12" t="s">
         <v>197</v>
       </c>
@@ -6907,7 +6947,7 @@
       <c r="T85" s="16">
         <v>2</v>
       </c>
-      <c r="U85" s="16">
+      <c r="U85" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V85" s="61">
@@ -6920,7 +6960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C86" s="12" t="s">
         <v>198</v>
       </c>
@@ -6957,7 +6997,7 @@
       <c r="T86" s="16">
         <v>10</v>
       </c>
-      <c r="U86" s="16">
+      <c r="U86" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V86" s="61">
@@ -6970,7 +7010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C87" s="12" t="s">
         <v>199</v>
       </c>
@@ -7007,7 +7047,7 @@
       <c r="T87" s="16">
         <v>10</v>
       </c>
-      <c r="U87" s="16">
+      <c r="U87" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V87" s="61">
@@ -7020,7 +7060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C88" s="12" t="s">
         <v>200</v>
       </c>
@@ -7057,7 +7097,7 @@
       <c r="T88" s="16">
         <v>2</v>
       </c>
-      <c r="U88" s="16">
+      <c r="U88" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V88" s="61">
@@ -7107,13 +7147,20 @@
       <c r="T89" s="16">
         <v>2</v>
       </c>
-      <c r="U89" s="16">
+      <c r="U89" s="67">
         <v>0.45624999999999999</v>
       </c>
-      <c r="V89" s="61"/>
-      <c r="W89" s="61"/>
-    </row>
-    <row r="90" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="V89" s="61">
+        <v>0</v>
+      </c>
+      <c r="W89" s="61">
+        <v>0</v>
+      </c>
+      <c r="X89" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C90" s="12" t="s">
         <v>202</v>
       </c>
@@ -7150,7 +7197,7 @@
       <c r="T90" s="16">
         <v>0</v>
       </c>
-      <c r="U90" s="16">
+      <c r="U90" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V90" s="61">
@@ -7163,7 +7210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C91" s="12" t="s">
         <v>205</v>
       </c>
@@ -7210,7 +7257,7 @@
       <c r="T91" s="16">
         <v>0</v>
       </c>
-      <c r="U91" s="16">
+      <c r="U91" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V91" s="61">
@@ -7223,7 +7270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C92" s="12" t="s">
         <v>149</v>
       </c>
@@ -7254,11 +7301,11 @@
       <c r="R92" s="16"/>
       <c r="S92" s="16"/>
       <c r="T92" s="16"/>
-      <c r="U92" s="16"/>
+      <c r="U92" s="67"/>
       <c r="V92" s="61"/>
       <c r="W92" s="61"/>
     </row>
-    <row r="93" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C93" s="12" t="s">
         <v>208</v>
       </c>
@@ -7305,7 +7352,7 @@
       <c r="T93" s="16">
         <v>0</v>
       </c>
-      <c r="U93" s="16">
+      <c r="U93" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V93" s="61">
@@ -7318,7 +7365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C94" s="12" t="s">
         <v>149</v>
       </c>
@@ -7349,11 +7396,11 @@
       <c r="R94" s="16"/>
       <c r="S94" s="16"/>
       <c r="T94" s="16"/>
-      <c r="U94" s="16"/>
+      <c r="U94" s="67"/>
       <c r="V94" s="61"/>
       <c r="W94" s="61"/>
     </row>
-    <row r="95" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C95" s="12" t="s">
         <v>210</v>
       </c>
@@ -7390,7 +7437,7 @@
       <c r="T95" s="16">
         <v>0</v>
       </c>
-      <c r="U95" s="16">
+      <c r="U95" s="67">
         <v>0.34218799999999999</v>
       </c>
       <c r="V95" s="61">
@@ -7403,7 +7450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C96" s="12" t="s">
         <v>212</v>
       </c>
@@ -7448,7 +7495,7 @@
       <c r="T96" s="16">
         <v>0</v>
       </c>
-      <c r="U96" s="16">
+      <c r="U96" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V96" s="61">
@@ -7461,7 +7508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C97" s="12" t="s">
         <v>213</v>
       </c>
@@ -7506,7 +7553,7 @@
       <c r="T97" s="16">
         <v>0</v>
       </c>
-      <c r="U97" s="16">
+      <c r="U97" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V97" s="61">
@@ -7519,7 +7566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C98" s="12" t="s">
         <v>214</v>
       </c>
@@ -7556,7 +7603,7 @@
       <c r="T98" s="16">
         <v>0</v>
       </c>
-      <c r="U98" s="16">
+      <c r="U98" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V98" s="61">
@@ -7569,7 +7616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C99" s="12" t="s">
         <v>216</v>
       </c>
@@ -7606,7 +7653,7 @@
       <c r="T99" s="16">
         <v>0</v>
       </c>
-      <c r="U99" s="16">
+      <c r="U99" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V99" s="61">
@@ -7619,7 +7666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C100" s="12" t="s">
         <v>218</v>
       </c>
@@ -7656,7 +7703,7 @@
       <c r="T100" s="16">
         <v>0</v>
       </c>
-      <c r="U100" s="16">
+      <c r="U100" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V100" s="61">
@@ -7669,7 +7716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C101" s="12" t="s">
         <v>220</v>
       </c>
@@ -7706,7 +7753,7 @@
       <c r="T101" s="16">
         <v>0</v>
       </c>
-      <c r="U101" s="16">
+      <c r="U101" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V101" s="61">
@@ -7719,7 +7766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C102" s="12" t="s">
         <v>222</v>
       </c>
@@ -7756,7 +7803,7 @@
       <c r="T102" s="16">
         <v>0</v>
       </c>
-      <c r="U102" s="16">
+      <c r="U102" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V102" s="61">
@@ -7769,7 +7816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C103" s="12" t="s">
         <v>224</v>
       </c>
@@ -7806,7 +7853,7 @@
       <c r="T103" s="16">
         <v>0</v>
       </c>
-      <c r="U103" s="16">
+      <c r="U103" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V103" s="61">
@@ -7819,7 +7866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C104" s="12" t="s">
         <v>226</v>
       </c>
@@ -7856,7 +7903,7 @@
       <c r="T104" s="16">
         <v>0</v>
       </c>
-      <c r="U104" s="16">
+      <c r="U104" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V104" s="61">
@@ -7869,7 +7916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C105" s="12" t="s">
         <v>227</v>
       </c>
@@ -7906,7 +7953,7 @@
       <c r="T105" s="16">
         <v>7</v>
       </c>
-      <c r="U105" s="16">
+      <c r="U105" s="67">
         <v>0.05</v>
       </c>
       <c r="V105" s="61">
@@ -7919,7 +7966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C106" s="12" t="s">
         <v>230</v>
       </c>
@@ -7956,7 +8003,7 @@
       <c r="T106" s="16">
         <v>7</v>
       </c>
-      <c r="U106" s="16">
+      <c r="U106" s="67">
         <v>0.05</v>
       </c>
       <c r="V106" s="61">
@@ -7969,7 +8016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C107" s="12" t="s">
         <v>232</v>
       </c>
@@ -8006,7 +8053,7 @@
       <c r="T107" s="16">
         <v>7</v>
       </c>
-      <c r="U107" s="16">
+      <c r="U107" s="67">
         <v>0.05</v>
       </c>
       <c r="V107" s="61">
@@ -8019,7 +8066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C108" s="12" t="s">
         <v>234</v>
       </c>
@@ -8056,7 +8103,7 @@
       <c r="T108" s="16">
         <v>0</v>
       </c>
-      <c r="U108" s="16">
+      <c r="U108" s="67">
         <v>0.05</v>
       </c>
       <c r="V108" s="61">
@@ -8114,7 +8161,7 @@
       <c r="T109" s="16">
         <v>2</v>
       </c>
-      <c r="U109" s="16">
+      <c r="U109" s="67">
         <v>0.05</v>
       </c>
       <c r="V109" s="61">
@@ -8127,7 +8174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C110" s="12" t="s">
         <v>238</v>
       </c>
@@ -8164,13 +8211,13 @@
       <c r="T110" s="16">
         <v>5</v>
       </c>
-      <c r="U110" s="16">
+      <c r="U110" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V110" s="61"/>
       <c r="W110" s="61"/>
     </row>
-    <row r="111" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C111" s="12" t="s">
         <v>241</v>
       </c>
@@ -8207,13 +8254,13 @@
       <c r="T111" s="16">
         <v>5</v>
       </c>
-      <c r="U111" s="16">
+      <c r="U111" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V111" s="61"/>
       <c r="W111" s="61"/>
     </row>
-    <row r="112" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C112" s="12" t="s">
         <v>243</v>
       </c>
@@ -8250,13 +8297,13 @@
       <c r="T112" s="16">
         <v>5</v>
       </c>
-      <c r="U112" s="16">
+      <c r="U112" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V112" s="61"/>
       <c r="W112" s="61"/>
     </row>
-    <row r="113" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C113" s="12" t="s">
         <v>245</v>
       </c>
@@ -8297,7 +8344,7 @@
       <c r="T113" s="16">
         <v>0</v>
       </c>
-      <c r="U113" s="16">
+      <c r="U113" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V113" s="61"/>
@@ -8348,13 +8395,13 @@
       <c r="T114" s="16">
         <v>2</v>
       </c>
-      <c r="U114" s="16">
+      <c r="U114" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V114" s="61"/>
       <c r="W114" s="61"/>
     </row>
-    <row r="115" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C115" s="12" t="s">
         <v>249</v>
       </c>
@@ -8391,13 +8438,13 @@
       <c r="T115" s="16">
         <v>5</v>
       </c>
-      <c r="U115" s="16">
+      <c r="U115" s="67">
         <v>0.45624999999999999</v>
       </c>
       <c r="V115" s="61"/>
       <c r="W115" s="61"/>
     </row>
-    <row r="116" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C116" s="12" t="s">
         <v>550</v>
       </c>
@@ -8442,13 +8489,13 @@
       <c r="T116" s="16">
         <v>0</v>
       </c>
-      <c r="U116" s="16">
+      <c r="U116" s="67">
         <v>0.22812499999999999</v>
       </c>
       <c r="V116" s="61"/>
       <c r="W116" s="61"/>
     </row>
-    <row r="117" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C117" s="12" t="s">
         <v>551</v>
       </c>
@@ -8493,13 +8540,13 @@
       <c r="T117" s="16">
         <v>0</v>
       </c>
-      <c r="U117" s="16">
+      <c r="U117" s="67">
         <v>0.22812499999999999</v>
       </c>
       <c r="V117" s="61"/>
       <c r="W117" s="61"/>
     </row>
-    <row r="118" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C118" s="12" t="s">
         <v>149</v>
       </c>
@@ -8524,11 +8571,11 @@
       <c r="R118" s="16"/>
       <c r="S118" s="16"/>
       <c r="T118" s="16"/>
-      <c r="U118" s="16"/>
+      <c r="U118" s="67"/>
       <c r="V118" s="61"/>
       <c r="W118" s="61"/>
     </row>
-    <row r="119" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C119" s="12" t="s">
         <v>254</v>
       </c>
@@ -8569,13 +8616,13 @@
       <c r="T119" s="16">
         <v>0</v>
       </c>
-      <c r="U119" s="16">
+      <c r="U119" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V119" s="61"/>
       <c r="W119" s="61"/>
     </row>
-    <row r="120" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C120" s="12" t="s">
         <v>257</v>
       </c>
@@ -8612,13 +8659,13 @@
       <c r="T120" s="16">
         <v>0</v>
       </c>
-      <c r="U120" s="16">
+      <c r="U120" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V120" s="65"/>
       <c r="W120" s="61"/>
     </row>
-    <row r="121" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C121" s="12" t="s">
         <v>260</v>
       </c>
@@ -8655,13 +8702,13 @@
       <c r="T121" s="16">
         <v>0</v>
       </c>
-      <c r="U121" s="16">
+      <c r="U121" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V121" s="65"/>
       <c r="W121" s="61"/>
     </row>
-    <row r="122" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C122" s="12" t="s">
         <v>262</v>
       </c>
@@ -8702,13 +8749,13 @@
       <c r="T122" s="16">
         <v>0</v>
       </c>
-      <c r="U122" s="16">
+      <c r="U122" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V122" s="61"/>
       <c r="W122" s="61"/>
     </row>
-    <row r="123" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C123" s="12" t="s">
         <v>264</v>
       </c>
@@ -8745,8 +8792,8 @@
       <c r="T123" s="16">
         <v>15</v>
       </c>
-      <c r="U123" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U123" s="67">
+        <v>0.1</v>
       </c>
       <c r="V123" s="61">
         <v>1.12E-2</v>
@@ -8758,7 +8805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C124" s="12" t="s">
         <v>267</v>
       </c>
@@ -8795,8 +8842,8 @@
       <c r="T124" s="16">
         <v>3</v>
       </c>
-      <c r="U124" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U124" s="67">
+        <v>0.1</v>
       </c>
       <c r="V124" s="61">
         <v>0.1</v>
@@ -8808,7 +8855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C125" s="12" t="s">
         <v>269</v>
       </c>
@@ -8845,8 +8892,8 @@
       <c r="T125" s="16">
         <v>3</v>
       </c>
-      <c r="U125" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U125" s="67">
+        <v>0.1</v>
       </c>
       <c r="V125" s="61">
         <v>6.4000000000000003E-3</v>
@@ -8858,7 +8905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C126" s="12" t="s">
         <v>271</v>
       </c>
@@ -8895,8 +8942,8 @@
       <c r="T126" s="16">
         <v>2</v>
       </c>
-      <c r="U126" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U126" s="67">
+        <v>0.1</v>
       </c>
       <c r="V126" s="61">
         <v>0.1</v>
@@ -8908,7 +8955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C127" s="12" t="s">
         <v>273</v>
       </c>
@@ -8945,8 +8992,8 @@
       <c r="T127" s="16">
         <v>2</v>
       </c>
-      <c r="U127" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U127" s="67">
+        <v>0.1</v>
       </c>
       <c r="V127" s="61">
         <v>0.23910000000000001</v>
@@ -8958,7 +9005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C128" s="12" t="s">
         <v>275</v>
       </c>
@@ -8995,8 +9042,8 @@
       <c r="T128" s="16">
         <v>10</v>
       </c>
-      <c r="U128" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U128" s="67">
+        <v>0.1</v>
       </c>
       <c r="V128" s="61">
         <v>0.1</v>
@@ -9008,7 +9055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C129" s="12" t="s">
         <v>277</v>
       </c>
@@ -9045,8 +9092,8 @@
       <c r="T129" s="16">
         <v>10</v>
       </c>
-      <c r="U129" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U129" s="67">
+        <v>0.1</v>
       </c>
       <c r="V129" s="61">
         <v>0.1</v>
@@ -9058,7 +9105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C130" s="12" t="s">
         <v>279</v>
       </c>
@@ -9095,8 +9142,8 @@
       <c r="T130" s="16">
         <v>2</v>
       </c>
-      <c r="U130" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U130" s="67">
+        <v>0.1</v>
       </c>
       <c r="V130" s="61">
         <v>0.1</v>
@@ -9108,7 +9155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C131" s="12" t="s">
         <v>281</v>
       </c>
@@ -9145,8 +9192,8 @@
       <c r="T131" s="16">
         <v>2</v>
       </c>
-      <c r="U131" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U131" s="67">
+        <v>0.1</v>
       </c>
       <c r="V131" s="61">
         <v>0</v>
@@ -9195,20 +9242,20 @@
       <c r="T132" s="16">
         <v>2</v>
       </c>
-      <c r="U132" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U132" s="67">
+        <v>0.1</v>
       </c>
       <c r="V132" s="61">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="W132" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X132" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C133" s="12" t="s">
         <v>285</v>
       </c>
@@ -9245,7 +9292,7 @@
       <c r="T133" s="16">
         <v>15</v>
       </c>
-      <c r="U133" s="16">
+      <c r="U133" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V133" s="61">
@@ -9258,7 +9305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C134" s="12" t="s">
         <v>287</v>
       </c>
@@ -9295,7 +9342,7 @@
       <c r="T134" s="16">
         <v>3</v>
       </c>
-      <c r="U134" s="16">
+      <c r="U134" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V134" s="61">
@@ -9308,7 +9355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C135" s="12" t="s">
         <v>288</v>
       </c>
@@ -9345,7 +9392,7 @@
       <c r="T135" s="16">
         <v>3</v>
       </c>
-      <c r="U135" s="16">
+      <c r="U135" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V135" s="61">
@@ -9358,7 +9405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C136" s="12" t="s">
         <v>289</v>
       </c>
@@ -9395,7 +9442,7 @@
       <c r="T136" s="16">
         <v>2</v>
       </c>
-      <c r="U136" s="16">
+      <c r="U136" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V136" s="61">
@@ -9408,7 +9455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C137" s="12" t="s">
         <v>290</v>
       </c>
@@ -9445,7 +9492,7 @@
       <c r="T137" s="16">
         <v>2</v>
       </c>
-      <c r="U137" s="16">
+      <c r="U137" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V137" s="61">
@@ -9458,7 +9505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C138" s="12" t="s">
         <v>291</v>
       </c>
@@ -9495,7 +9542,7 @@
       <c r="T138" s="16">
         <v>10</v>
       </c>
-      <c r="U138" s="16">
+      <c r="U138" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V138" s="61">
@@ -9508,7 +9555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C139" s="12" t="s">
         <v>292</v>
       </c>
@@ -9545,7 +9592,7 @@
       <c r="T139" s="16">
         <v>10</v>
       </c>
-      <c r="U139" s="16">
+      <c r="U139" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V139" s="61">
@@ -9558,7 +9605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C140" s="12" t="s">
         <v>293</v>
       </c>
@@ -9595,7 +9642,7 @@
       <c r="T140" s="16">
         <v>2</v>
       </c>
-      <c r="U140" s="16">
+      <c r="U140" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V140" s="61">
@@ -9608,7 +9655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C141" s="12" t="s">
         <v>294</v>
       </c>
@@ -9645,7 +9692,7 @@
       <c r="T141" s="16">
         <v>2</v>
       </c>
-      <c r="U141" s="16">
+      <c r="U141" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V141" s="61">
@@ -9695,20 +9742,20 @@
       <c r="T142" s="16">
         <v>2</v>
       </c>
-      <c r="U142" s="16">
+      <c r="U142" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V142" s="61">
         <v>0</v>
       </c>
       <c r="W142" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X142" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C143" s="12" t="s">
         <v>296</v>
       </c>
@@ -9755,8 +9802,8 @@
       <c r="T143" s="16">
         <v>0</v>
       </c>
-      <c r="U143" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U143" s="67">
+        <v>0.1</v>
       </c>
       <c r="V143" s="61">
         <v>0.8</v>
@@ -9768,7 +9815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C144" s="12" t="s">
         <v>149</v>
       </c>
@@ -9799,11 +9846,11 @@
       <c r="R144" s="16"/>
       <c r="S144" s="16"/>
       <c r="T144" s="16"/>
-      <c r="U144" s="16"/>
+      <c r="U144" s="67"/>
       <c r="V144" s="61"/>
       <c r="W144" s="61"/>
     </row>
-    <row r="145" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C145" s="12" t="s">
         <v>299</v>
       </c>
@@ -9850,8 +9897,8 @@
       <c r="T145" s="16">
         <v>0</v>
       </c>
-      <c r="U145" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U145" s="67">
+        <v>0.1</v>
       </c>
       <c r="V145" s="61">
         <v>0.8</v>
@@ -9863,7 +9910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C146" s="12" t="s">
         <v>149</v>
       </c>
@@ -9894,11 +9941,11 @@
       <c r="R146" s="16"/>
       <c r="S146" s="16"/>
       <c r="T146" s="16"/>
-      <c r="U146" s="16"/>
+      <c r="U146" s="67"/>
       <c r="V146" s="61"/>
       <c r="W146" s="61"/>
     </row>
-    <row r="147" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C147" s="12" t="s">
         <v>301</v>
       </c>
@@ -9935,8 +9982,8 @@
       <c r="T147" s="16">
         <v>0</v>
       </c>
-      <c r="U147" s="16">
-        <v>0.33565699999999998</v>
+      <c r="U147" s="67">
+        <v>0.1</v>
       </c>
       <c r="V147" s="61">
         <v>0.3</v>
@@ -9948,7 +9995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C148" s="12" t="s">
         <v>303</v>
       </c>
@@ -9993,7 +10040,7 @@
       <c r="T148" s="16">
         <v>0</v>
       </c>
-      <c r="U148" s="16">
+      <c r="U148" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V148" s="61">
@@ -10006,7 +10053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C149" s="12" t="s">
         <v>304</v>
       </c>
@@ -10051,7 +10098,7 @@
       <c r="T149" s="16">
         <v>0</v>
       </c>
-      <c r="U149" s="16">
+      <c r="U149" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V149" s="61">
@@ -10064,7 +10111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C150" s="12" t="s">
         <v>305</v>
       </c>
@@ -10101,7 +10148,7 @@
       <c r="T150" s="16">
         <v>0</v>
       </c>
-      <c r="U150" s="16">
+      <c r="U150" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V150" s="61">
@@ -10114,7 +10161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C151" s="12" t="s">
         <v>307</v>
       </c>
@@ -10151,7 +10198,7 @@
       <c r="T151" s="16">
         <v>0</v>
       </c>
-      <c r="U151" s="16">
+      <c r="U151" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V151" s="61">
@@ -10164,7 +10211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C152" s="12" t="s">
         <v>309</v>
       </c>
@@ -10201,7 +10248,7 @@
       <c r="T152" s="16">
         <v>0</v>
       </c>
-      <c r="U152" s="16">
+      <c r="U152" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V152" s="61">
@@ -10214,7 +10261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C153" s="12" t="s">
         <v>311</v>
       </c>
@@ -10251,7 +10298,7 @@
       <c r="T153" s="16">
         <v>0</v>
       </c>
-      <c r="U153" s="16">
+      <c r="U153" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V153" s="61">
@@ -10264,7 +10311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C154" s="12" t="s">
         <v>313</v>
       </c>
@@ -10301,7 +10348,7 @@
       <c r="T154" s="16">
         <v>0</v>
       </c>
-      <c r="U154" s="16">
+      <c r="U154" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V154" s="61">
@@ -10314,7 +10361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C155" s="12" t="s">
         <v>315</v>
       </c>
@@ -10351,7 +10398,7 @@
       <c r="T155" s="16">
         <v>0</v>
       </c>
-      <c r="U155" s="16">
+      <c r="U155" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V155" s="61">
@@ -10364,7 +10411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C156" s="12" t="s">
         <v>317</v>
       </c>
@@ -10401,13 +10448,13 @@
       <c r="T156" s="16">
         <v>7</v>
       </c>
-      <c r="U156" s="16">
+      <c r="U156" s="67">
         <v>0.1</v>
       </c>
       <c r="V156" s="61"/>
       <c r="W156" s="61"/>
     </row>
-    <row r="157" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C157" s="12" t="s">
         <v>320</v>
       </c>
@@ -10444,13 +10491,13 @@
       <c r="T157" s="16">
         <v>7</v>
       </c>
-      <c r="U157" s="16">
+      <c r="U157" s="67">
         <v>0.1</v>
       </c>
       <c r="V157" s="61"/>
       <c r="W157" s="61"/>
     </row>
-    <row r="158" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C158" s="12" t="s">
         <v>322</v>
       </c>
@@ -10487,13 +10534,13 @@
       <c r="T158" s="16">
         <v>7</v>
       </c>
-      <c r="U158" s="16">
+      <c r="U158" s="67">
         <v>0.1</v>
       </c>
       <c r="V158" s="61"/>
       <c r="W158" s="61"/>
     </row>
-    <row r="159" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C159" s="12" t="s">
         <v>324</v>
       </c>
@@ -10530,7 +10577,7 @@
       <c r="T159" s="16">
         <v>0</v>
       </c>
-      <c r="U159" s="16">
+      <c r="U159" s="67">
         <v>0.1</v>
       </c>
       <c r="V159" s="61"/>
@@ -10581,7 +10628,7 @@
       <c r="T160" s="16">
         <v>2</v>
       </c>
-      <c r="U160" s="16">
+      <c r="U160" s="67">
         <v>0.1</v>
       </c>
       <c r="V160" s="61">
@@ -10594,7 +10641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C161" s="12" t="s">
         <v>328</v>
       </c>
@@ -10631,13 +10678,13 @@
       <c r="T161" s="16">
         <v>5</v>
       </c>
-      <c r="U161" s="16">
+      <c r="U161" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V161" s="61"/>
       <c r="W161" s="61"/>
     </row>
-    <row r="162" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C162" s="12" t="s">
         <v>331</v>
       </c>
@@ -10674,13 +10721,13 @@
       <c r="T162" s="16">
         <v>5</v>
       </c>
-      <c r="U162" s="16">
+      <c r="U162" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V162" s="61"/>
       <c r="W162" s="61"/>
     </row>
-    <row r="163" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C163" s="12" t="s">
         <v>333</v>
       </c>
@@ -10717,13 +10764,13 @@
       <c r="T163" s="16">
         <v>5</v>
       </c>
-      <c r="U163" s="16">
+      <c r="U163" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V163" s="61"/>
       <c r="W163" s="61"/>
     </row>
-    <row r="164" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C164" s="12" t="s">
         <v>335</v>
       </c>
@@ -10764,7 +10811,7 @@
       <c r="T164" s="16">
         <v>0</v>
       </c>
-      <c r="U164" s="16">
+      <c r="U164" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V164" s="61"/>
@@ -10815,13 +10862,13 @@
       <c r="T165" s="16">
         <v>2</v>
       </c>
-      <c r="U165" s="16">
+      <c r="U165" s="67">
         <v>0.44754300000000002</v>
       </c>
       <c r="V165" s="61"/>
       <c r="W165" s="61"/>
     </row>
-    <row r="166" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C166" s="12" t="s">
         <v>552</v>
       </c>
@@ -10866,13 +10913,13 @@
       <c r="T166" s="16">
         <v>0</v>
       </c>
-      <c r="U166" s="16">
+      <c r="U166" s="67">
         <v>0.223772</v>
       </c>
       <c r="V166" s="61"/>
       <c r="W166" s="61"/>
     </row>
-    <row r="167" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C167" s="12" t="s">
         <v>553</v>
       </c>
@@ -10917,13 +10964,13 @@
       <c r="T167" s="16">
         <v>0</v>
       </c>
-      <c r="U167" s="16">
+      <c r="U167" s="67">
         <v>0.223772</v>
       </c>
       <c r="V167" s="61"/>
       <c r="W167" s="61"/>
     </row>
-    <row r="168" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C168" s="12" t="s">
         <v>149</v>
       </c>
@@ -10948,11 +10995,11 @@
       <c r="R168" s="16"/>
       <c r="S168" s="16"/>
       <c r="T168" s="16"/>
-      <c r="U168" s="16"/>
+      <c r="U168" s="67"/>
       <c r="V168" s="61"/>
       <c r="W168" s="61"/>
     </row>
-    <row r="169" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C169" s="12" t="s">
         <v>341</v>
       </c>
@@ -10993,13 +11040,13 @@
       <c r="T169" s="16">
         <v>0</v>
       </c>
-      <c r="U169" s="16">
+      <c r="U169" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V169" s="61"/>
       <c r="W169" s="61"/>
     </row>
-    <row r="170" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C170" s="12" t="s">
         <v>344</v>
       </c>
@@ -11036,13 +11083,13 @@
       <c r="T170" s="16">
         <v>0</v>
       </c>
-      <c r="U170" s="16">
+      <c r="U170" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V170" s="61"/>
       <c r="W170" s="61"/>
     </row>
-    <row r="171" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C171" s="12" t="s">
         <v>347</v>
       </c>
@@ -11079,13 +11126,13 @@
       <c r="T171" s="16">
         <v>0</v>
       </c>
-      <c r="U171" s="16">
+      <c r="U171" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V171" s="61"/>
       <c r="W171" s="61"/>
     </row>
-    <row r="172" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C172" s="12" t="s">
         <v>349</v>
       </c>
@@ -11122,13 +11169,13 @@
       <c r="T172" s="16">
         <v>0</v>
       </c>
-      <c r="U172" s="16">
+      <c r="U172" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V172" s="61"/>
       <c r="W172" s="61"/>
     </row>
-    <row r="173" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C173" s="12" t="s">
         <v>351</v>
       </c>
@@ -11165,7 +11212,7 @@
       <c r="T173" s="16">
         <v>0</v>
       </c>
-      <c r="U173" s="16">
+      <c r="U173" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V173" s="61"/>
@@ -11208,13 +11255,13 @@
       <c r="T174" s="16">
         <v>0</v>
       </c>
-      <c r="U174" s="16">
+      <c r="U174" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V174" s="61"/>
       <c r="W174" s="61"/>
     </row>
-    <row r="175" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C175" s="12" t="s">
         <v>355</v>
       </c>
@@ -11251,13 +11298,13 @@
       <c r="T175" s="16">
         <v>0</v>
       </c>
-      <c r="U175" s="16">
+      <c r="U175" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V175" s="61"/>
       <c r="W175" s="61"/>
     </row>
-    <row r="176" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C176" s="12" t="s">
         <v>357</v>
       </c>
@@ -11294,13 +11341,13 @@
       <c r="T176" s="16">
         <v>0</v>
       </c>
-      <c r="U176" s="16">
+      <c r="U176" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V176" s="61"/>
       <c r="W176" s="61"/>
     </row>
-    <row r="177" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C177" s="12" t="s">
         <v>359</v>
       </c>
@@ -11337,7 +11384,7 @@
       <c r="T177" s="16">
         <v>0</v>
       </c>
-      <c r="U177" s="16">
+      <c r="U177" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V177" s="61"/>
@@ -11380,13 +11427,13 @@
       <c r="T178" s="16">
         <v>0</v>
       </c>
-      <c r="U178" s="16">
+      <c r="U178" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V178" s="61"/>
       <c r="W178" s="61"/>
     </row>
-    <row r="179" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C179" s="12" t="s">
         <v>363</v>
       </c>
@@ -11423,13 +11470,13 @@
       <c r="T179" s="16">
         <v>0</v>
       </c>
-      <c r="U179" s="16">
+      <c r="U179" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V179" s="65"/>
       <c r="W179" s="61"/>
     </row>
-    <row r="180" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C180" s="12" t="s">
         <v>366</v>
       </c>
@@ -11466,13 +11513,13 @@
       <c r="T180" s="16">
         <v>0</v>
       </c>
-      <c r="U180" s="16">
+      <c r="U180" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V180" s="65"/>
       <c r="W180" s="61"/>
     </row>
-    <row r="181" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C181" s="12" t="s">
         <v>368</v>
       </c>
@@ -11513,13 +11560,13 @@
       <c r="T181" s="16">
         <v>0</v>
       </c>
-      <c r="U181" s="16">
+      <c r="U181" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V181" s="61"/>
       <c r="W181" s="61"/>
     </row>
-    <row r="182" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C182" s="12" t="s">
         <v>370</v>
       </c>
@@ -11556,8 +11603,8 @@
       <c r="T182" s="16">
         <v>15</v>
       </c>
-      <c r="U182" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U182" s="67">
+        <v>0.1</v>
       </c>
       <c r="V182" s="61">
         <v>0</v>
@@ -11569,7 +11616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C183" s="12" t="s">
         <v>373</v>
       </c>
@@ -11606,8 +11653,8 @@
       <c r="T183" s="16">
         <v>3</v>
       </c>
-      <c r="U183" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U183" s="67">
+        <v>0.1</v>
       </c>
       <c r="V183" s="61">
         <v>0</v>
@@ -11619,7 +11666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C184" s="12" t="s">
         <v>375</v>
       </c>
@@ -11656,8 +11703,8 @@
       <c r="T184" s="16">
         <v>3</v>
       </c>
-      <c r="U184" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U184" s="67">
+        <v>0.1</v>
       </c>
       <c r="V184" s="61">
         <v>0</v>
@@ -11669,7 +11716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C185" s="12" t="s">
         <v>377</v>
       </c>
@@ -11706,8 +11753,8 @@
       <c r="T185" s="16">
         <v>2</v>
       </c>
-      <c r="U185" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U185" s="67">
+        <v>0.1</v>
       </c>
       <c r="V185" s="61">
         <v>7.4999999999999997E-3</v>
@@ -11719,7 +11766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C186" s="12" t="s">
         <v>379</v>
       </c>
@@ -11756,8 +11803,8 @@
       <c r="T186" s="16">
         <v>2</v>
       </c>
-      <c r="U186" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U186" s="67">
+        <v>0.1</v>
       </c>
       <c r="V186" s="61">
         <v>0.15959999999999999</v>
@@ -11769,7 +11816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C187" s="12" t="s">
         <v>381</v>
       </c>
@@ -11806,8 +11853,8 @@
       <c r="T187" s="16">
         <v>10</v>
       </c>
-      <c r="U187" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U187" s="67">
+        <v>0.1</v>
       </c>
       <c r="V187" s="61">
         <v>0.05</v>
@@ -11819,7 +11866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C188" s="12" t="s">
         <v>383</v>
       </c>
@@ -11856,8 +11903,8 @@
       <c r="T188" s="16">
         <v>10</v>
       </c>
-      <c r="U188" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U188" s="67">
+        <v>0.1</v>
       </c>
       <c r="V188" s="61">
         <v>0.05</v>
@@ -11869,7 +11916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C189" s="12" t="s">
         <v>385</v>
       </c>
@@ -11906,8 +11953,8 @@
       <c r="T189" s="16">
         <v>2</v>
       </c>
-      <c r="U189" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U189" s="67">
+        <v>0.1</v>
       </c>
       <c r="V189" s="61">
         <v>0.1</v>
@@ -11919,7 +11966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C190" s="12" t="s">
         <v>387</v>
       </c>
@@ -11956,8 +12003,8 @@
       <c r="T190" s="16">
         <v>2</v>
       </c>
-      <c r="U190" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U190" s="67">
+        <v>0.1</v>
       </c>
       <c r="V190" s="61">
         <v>0</v>
@@ -12006,20 +12053,20 @@
       <c r="T191" s="16">
         <v>2</v>
       </c>
-      <c r="U191" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U191" s="67">
+        <v>0.1</v>
       </c>
       <c r="V191" s="61">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="W191" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X191" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C192" s="12" t="s">
         <v>391</v>
       </c>
@@ -12056,7 +12103,7 @@
       <c r="T192" s="16">
         <v>15</v>
       </c>
-      <c r="U192" s="16">
+      <c r="U192" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V192" s="61">
@@ -12069,7 +12116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C193" s="12" t="s">
         <v>393</v>
       </c>
@@ -12106,7 +12153,7 @@
       <c r="T193" s="16">
         <v>3</v>
       </c>
-      <c r="U193" s="16">
+      <c r="U193" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V193" s="61">
@@ -12119,7 +12166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C194" s="12" t="s">
         <v>394</v>
       </c>
@@ -12156,7 +12203,7 @@
       <c r="T194" s="16">
         <v>3</v>
       </c>
-      <c r="U194" s="16">
+      <c r="U194" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V194" s="61">
@@ -12169,7 +12216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C195" s="12" t="s">
         <v>395</v>
       </c>
@@ -12206,7 +12253,7 @@
       <c r="T195" s="16">
         <v>2</v>
       </c>
-      <c r="U195" s="16">
+      <c r="U195" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V195" s="61">
@@ -12219,7 +12266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C196" s="12" t="s">
         <v>396</v>
       </c>
@@ -12256,7 +12303,7 @@
       <c r="T196" s="16">
         <v>2</v>
       </c>
-      <c r="U196" s="16">
+      <c r="U196" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V196" s="61">
@@ -12269,7 +12316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C197" s="12" t="s">
         <v>397</v>
       </c>
@@ -12306,7 +12353,7 @@
       <c r="T197" s="16">
         <v>10</v>
       </c>
-      <c r="U197" s="16">
+      <c r="U197" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V197" s="61">
@@ -12319,7 +12366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C198" s="12" t="s">
         <v>398</v>
       </c>
@@ -12356,7 +12403,7 @@
       <c r="T198" s="16">
         <v>10</v>
       </c>
-      <c r="U198" s="16">
+      <c r="U198" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V198" s="61">
@@ -12369,7 +12416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C199" s="12" t="s">
         <v>399</v>
       </c>
@@ -12406,7 +12453,7 @@
       <c r="T199" s="16">
         <v>2</v>
       </c>
-      <c r="U199" s="16">
+      <c r="U199" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V199" s="61">
@@ -12419,7 +12466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C200" s="12" t="s">
         <v>400</v>
       </c>
@@ -12456,7 +12503,7 @@
       <c r="T200" s="16">
         <v>2</v>
       </c>
-      <c r="U200" s="16">
+      <c r="U200" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V200" s="61">
@@ -12506,20 +12553,20 @@
       <c r="T201" s="16">
         <v>2</v>
       </c>
-      <c r="U201" s="16">
+      <c r="U201" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V201" s="61">
         <v>0</v>
       </c>
       <c r="W201" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X201" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C202" s="12" t="s">
         <v>402</v>
       </c>
@@ -12556,7 +12603,7 @@
       <c r="T202" s="16">
         <v>0</v>
       </c>
-      <c r="U202" s="16">
+      <c r="U202" s="67">
         <v>0.36225000000000002</v>
       </c>
       <c r="V202" s="61">
@@ -12569,7 +12616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C203" s="12" t="s">
         <v>404</v>
       </c>
@@ -12616,8 +12663,8 @@
       <c r="T203" s="16">
         <v>0</v>
       </c>
-      <c r="U203" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U203" s="67">
+        <v>0.1</v>
       </c>
       <c r="V203" s="61">
         <v>0.7</v>
@@ -12629,7 +12676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C204" s="12" t="s">
         <v>149</v>
       </c>
@@ -12660,11 +12707,11 @@
       <c r="R204" s="16"/>
       <c r="S204" s="16"/>
       <c r="T204" s="16"/>
-      <c r="U204" s="16"/>
+      <c r="U204" s="67"/>
       <c r="V204" s="61"/>
       <c r="W204" s="61"/>
     </row>
-    <row r="205" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C205" s="12" t="s">
         <v>407</v>
       </c>
@@ -12711,8 +12758,8 @@
       <c r="T205" s="16">
         <v>0</v>
       </c>
-      <c r="U205" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U205" s="67">
+        <v>0.1</v>
       </c>
       <c r="V205" s="61">
         <v>0.7</v>
@@ -12724,7 +12771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C206" s="12" t="s">
         <v>149</v>
       </c>
@@ -12755,11 +12802,11 @@
       <c r="R206" s="16"/>
       <c r="S206" s="16"/>
       <c r="T206" s="16"/>
-      <c r="U206" s="16"/>
+      <c r="U206" s="67"/>
       <c r="V206" s="61"/>
       <c r="W206" s="61"/>
     </row>
-    <row r="207" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C207" s="12" t="s">
         <v>409</v>
       </c>
@@ -12796,8 +12843,8 @@
       <c r="T207" s="16">
         <v>0</v>
       </c>
-      <c r="U207" s="16">
-        <v>0.36225000000000002</v>
+      <c r="U207" s="67">
+        <v>0.1</v>
       </c>
       <c r="V207" s="61">
         <v>0.5</v>
@@ -12809,7 +12856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C208" s="12" t="s">
         <v>411</v>
       </c>
@@ -12854,7 +12901,7 @@
       <c r="T208" s="16">
         <v>0</v>
       </c>
-      <c r="U208" s="16">
+      <c r="U208" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V208" s="61">
@@ -12867,7 +12914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C209" s="12" t="s">
         <v>412</v>
       </c>
@@ -12912,7 +12959,7 @@
       <c r="T209" s="16">
         <v>0</v>
       </c>
-      <c r="U209" s="16">
+      <c r="U209" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V209" s="61">
@@ -12925,7 +12972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C210" s="12" t="s">
         <v>413</v>
       </c>
@@ -12962,7 +13009,7 @@
       <c r="T210" s="16">
         <v>0</v>
       </c>
-      <c r="U210" s="16">
+      <c r="U210" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V210" s="61">
@@ -12975,7 +13022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C211" s="12" t="s">
         <v>415</v>
       </c>
@@ -13012,7 +13059,7 @@
       <c r="T211" s="16">
         <v>0</v>
       </c>
-      <c r="U211" s="16">
+      <c r="U211" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V211" s="61">
@@ -13025,7 +13072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C212" s="12" t="s">
         <v>417</v>
       </c>
@@ -13062,7 +13109,7 @@
       <c r="T212" s="16">
         <v>0</v>
       </c>
-      <c r="U212" s="16">
+      <c r="U212" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V212" s="61">
@@ -13075,7 +13122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C213" s="12" t="s">
         <v>419</v>
       </c>
@@ -13112,7 +13159,7 @@
       <c r="T213" s="16">
         <v>2</v>
       </c>
-      <c r="U213" s="16">
+      <c r="U213" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V213" s="61">
@@ -13125,7 +13172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C214" s="12" t="s">
         <v>421</v>
       </c>
@@ -13162,7 +13209,7 @@
       <c r="T214" s="16">
         <v>2</v>
       </c>
-      <c r="U214" s="16">
+      <c r="U214" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V214" s="61">
@@ -13175,7 +13222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C215" s="12" t="s">
         <v>423</v>
       </c>
@@ -13212,7 +13259,7 @@
       <c r="T215" s="16">
         <v>2</v>
       </c>
-      <c r="U215" s="16">
+      <c r="U215" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V215" s="61">
@@ -13225,7 +13272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C216" s="12" t="s">
         <v>425</v>
       </c>
@@ -13262,7 +13309,7 @@
       <c r="T216" s="16">
         <v>7</v>
       </c>
-      <c r="U216" s="16">
+      <c r="U216" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V216" s="61">
@@ -13275,7 +13322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C217" s="12" t="s">
         <v>428</v>
       </c>
@@ -13312,7 +13359,7 @@
       <c r="T217" s="16">
         <v>7</v>
       </c>
-      <c r="U217" s="16">
+      <c r="U217" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V217" s="61">
@@ -13325,7 +13372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C218" s="12" t="s">
         <v>430</v>
       </c>
@@ -13362,7 +13409,7 @@
       <c r="T218" s="16">
         <v>7</v>
       </c>
-      <c r="U218" s="16">
+      <c r="U218" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V218" s="61">
@@ -13375,7 +13422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C219" s="12" t="s">
         <v>432</v>
       </c>
@@ -13412,7 +13459,7 @@
       <c r="T219" s="16">
         <v>0</v>
       </c>
-      <c r="U219" s="16">
+      <c r="U219" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V219" s="61">
@@ -13470,7 +13517,7 @@
       <c r="T220" s="16">
         <v>2</v>
       </c>
-      <c r="U220" s="16">
+      <c r="U220" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V220" s="61">
@@ -13483,7 +13530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C221" s="12" t="s">
         <v>436</v>
       </c>
@@ -13520,13 +13567,13 @@
       <c r="T221" s="16">
         <v>5</v>
       </c>
-      <c r="U221" s="16">
+      <c r="U221" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V221" s="61"/>
       <c r="W221" s="61"/>
     </row>
-    <row r="222" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C222" s="12" t="s">
         <v>439</v>
       </c>
@@ -13563,13 +13610,13 @@
       <c r="T222" s="16">
         <v>5</v>
       </c>
-      <c r="U222" s="16">
+      <c r="U222" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V222" s="61"/>
       <c r="W222" s="61"/>
     </row>
-    <row r="223" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C223" s="12" t="s">
         <v>441</v>
       </c>
@@ -13606,13 +13653,13 @@
       <c r="T223" s="16">
         <v>5</v>
       </c>
-      <c r="U223" s="16">
+      <c r="U223" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V223" s="61"/>
       <c r="W223" s="61"/>
     </row>
-    <row r="224" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C224" s="12" t="s">
         <v>443</v>
       </c>
@@ -13653,7 +13700,7 @@
       <c r="T224" s="16">
         <v>0</v>
       </c>
-      <c r="U224" s="16">
+      <c r="U224" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V224" s="61"/>
@@ -13704,13 +13751,13 @@
       <c r="T225" s="16">
         <v>2</v>
       </c>
-      <c r="U225" s="16">
+      <c r="U225" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V225" s="61"/>
       <c r="W225" s="61"/>
     </row>
-    <row r="226" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C226" s="12" t="s">
         <v>447</v>
       </c>
@@ -13747,13 +13794,13 @@
       <c r="T226" s="16">
         <v>5</v>
       </c>
-      <c r="U226" s="16">
+      <c r="U226" s="67">
         <v>0.48299999999999998</v>
       </c>
       <c r="V226" s="61"/>
       <c r="W226" s="61"/>
     </row>
-    <row r="227" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C227" s="12" t="s">
         <v>554</v>
       </c>
@@ -13798,13 +13845,13 @@
       <c r="T227" s="16">
         <v>0</v>
       </c>
-      <c r="U227" s="16">
+      <c r="U227" s="67">
         <v>0.24149999999999999</v>
       </c>
       <c r="V227" s="61"/>
       <c r="W227" s="61"/>
     </row>
-    <row r="228" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C228" s="12" t="s">
         <v>555</v>
       </c>
@@ -13849,13 +13896,13 @@
       <c r="T228" s="16">
         <v>0</v>
       </c>
-      <c r="U228" s="16">
+      <c r="U228" s="67">
         <v>0.24149999999999999</v>
       </c>
       <c r="V228" s="61"/>
       <c r="W228" s="61"/>
     </row>
-    <row r="229" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C229" s="12" t="s">
         <v>149</v>
       </c>
@@ -13880,11 +13927,11 @@
       <c r="R229" s="16"/>
       <c r="S229" s="16"/>
       <c r="T229" s="16"/>
-      <c r="U229" s="16"/>
+      <c r="U229" s="67"/>
       <c r="V229" s="61"/>
       <c r="W229" s="61"/>
     </row>
-    <row r="230" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C230" s="12" t="s">
         <v>452</v>
       </c>
@@ -13925,13 +13972,13 @@
       <c r="T230" s="16">
         <v>0</v>
       </c>
-      <c r="U230" s="16">
+      <c r="U230" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V230" s="61"/>
       <c r="W230" s="61"/>
     </row>
-    <row r="231" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C231" s="12" t="s">
         <v>455</v>
       </c>
@@ -13968,13 +14015,13 @@
       <c r="T231" s="16">
         <v>0</v>
       </c>
-      <c r="U231" s="16">
+      <c r="U231" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V231" s="64"/>
       <c r="W231" s="61"/>
     </row>
-    <row r="232" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C232" s="12" t="s">
         <v>458</v>
       </c>
@@ -14011,13 +14058,13 @@
       <c r="T232" s="16">
         <v>0</v>
       </c>
-      <c r="U232" s="16">
+      <c r="U232" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V232" s="65"/>
       <c r="W232" s="61"/>
     </row>
-    <row r="233" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C233" s="12" t="s">
         <v>460</v>
       </c>
@@ -14058,13 +14105,13 @@
       <c r="T233" s="16">
         <v>0</v>
       </c>
-      <c r="U233" s="16">
+      <c r="U233" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V233" s="65"/>
       <c r="W233" s="61"/>
     </row>
-    <row r="234" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C234" s="12" t="s">
         <v>462</v>
       </c>
@@ -14101,8 +14148,8 @@
       <c r="T234" s="16">
         <v>15</v>
       </c>
-      <c r="U234" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U234" s="67">
+        <v>0.1</v>
       </c>
       <c r="V234" s="61">
         <v>1</v>
@@ -14114,7 +14161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C235" s="12" t="s">
         <v>465</v>
       </c>
@@ -14151,8 +14198,8 @@
       <c r="T235" s="16">
         <v>3</v>
       </c>
-      <c r="U235" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U235" s="67">
+        <v>0.1</v>
       </c>
       <c r="V235" s="61">
         <v>9.9699999999999997E-2</v>
@@ -14164,7 +14211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C236" s="12" t="s">
         <v>467</v>
       </c>
@@ -14201,8 +14248,8 @@
       <c r="T236" s="16">
         <v>3</v>
       </c>
-      <c r="U236" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U236" s="67">
+        <v>0.1</v>
       </c>
       <c r="V236" s="61">
         <v>3.5000000000000001E-3</v>
@@ -14214,7 +14261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C237" s="12" t="s">
         <v>469</v>
       </c>
@@ -14251,8 +14298,8 @@
       <c r="T237" s="16">
         <v>2</v>
       </c>
-      <c r="U237" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U237" s="67">
+        <v>0.1</v>
       </c>
       <c r="V237" s="61">
         <v>0</v>
@@ -14264,7 +14311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C238" s="12" t="s">
         <v>471</v>
       </c>
@@ -14301,8 +14348,8 @@
       <c r="T238" s="16">
         <v>2</v>
       </c>
-      <c r="U238" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U238" s="67">
+        <v>0.1</v>
       </c>
       <c r="V238" s="61">
         <v>0.4118</v>
@@ -14314,7 +14361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C239" s="12" t="s">
         <v>473</v>
       </c>
@@ -14351,8 +14398,8 @@
       <c r="T239" s="16">
         <v>10</v>
       </c>
-      <c r="U239" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U239" s="67">
+        <v>0.1</v>
       </c>
       <c r="V239" s="61">
         <v>0.1</v>
@@ -14364,7 +14411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C240" s="12" t="s">
         <v>475</v>
       </c>
@@ -14401,8 +14448,8 @@
       <c r="T240" s="16">
         <v>10</v>
       </c>
-      <c r="U240" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U240" s="67">
+        <v>0.1</v>
       </c>
       <c r="V240" s="61">
         <v>0.1</v>
@@ -14414,7 +14461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C241" s="12" t="s">
         <v>477</v>
       </c>
@@ -14451,8 +14498,8 @@
       <c r="T241" s="16">
         <v>2</v>
       </c>
-      <c r="U241" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U241" s="67">
+        <v>0.1</v>
       </c>
       <c r="V241" s="61">
         <v>0.1</v>
@@ -14464,7 +14511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C242" s="12" t="s">
         <v>479</v>
       </c>
@@ -14501,8 +14548,8 @@
       <c r="T242" s="16">
         <v>2</v>
       </c>
-      <c r="U242" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U242" s="67">
+        <v>0.1</v>
       </c>
       <c r="V242" s="61">
         <v>0</v>
@@ -14551,20 +14598,20 @@
       <c r="T243" s="16">
         <v>2</v>
       </c>
-      <c r="U243" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U243" s="67">
+        <v>0.1</v>
       </c>
       <c r="V243" s="61">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="W243" s="61">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X243" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C244" s="12" t="s">
         <v>483</v>
       </c>
@@ -14601,7 +14648,7 @@
       <c r="T244" s="16">
         <v>15</v>
       </c>
-      <c r="U244" s="16">
+      <c r="U244" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V244" s="61">
@@ -14614,7 +14661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C245" s="12" t="s">
         <v>485</v>
       </c>
@@ -14651,7 +14698,7 @@
       <c r="T245" s="16">
         <v>3</v>
       </c>
-      <c r="U245" s="16">
+      <c r="U245" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V245" s="61">
@@ -14664,7 +14711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C246" s="12" t="s">
         <v>486</v>
       </c>
@@ -14701,7 +14748,7 @@
       <c r="T246" s="16">
         <v>3</v>
       </c>
-      <c r="U246" s="16">
+      <c r="U246" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V246" s="61">
@@ -14714,7 +14761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C247" s="12" t="s">
         <v>487</v>
       </c>
@@ -14751,7 +14798,7 @@
       <c r="T247" s="16">
         <v>2</v>
       </c>
-      <c r="U247" s="16">
+      <c r="U247" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V247" s="61">
@@ -14764,7 +14811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C248" s="12" t="s">
         <v>488</v>
       </c>
@@ -14801,7 +14848,7 @@
       <c r="T248" s="16">
         <v>2</v>
       </c>
-      <c r="U248" s="16">
+      <c r="U248" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V248" s="61">
@@ -14814,7 +14861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C249" s="12" t="s">
         <v>489</v>
       </c>
@@ -14851,7 +14898,7 @@
       <c r="T249" s="16">
         <v>10</v>
       </c>
-      <c r="U249" s="16">
+      <c r="U249" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V249" s="61">
@@ -14864,7 +14911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C250" s="12" t="s">
         <v>490</v>
       </c>
@@ -14901,7 +14948,7 @@
       <c r="T250" s="16">
         <v>10</v>
       </c>
-      <c r="U250" s="16">
+      <c r="U250" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V250" s="61">
@@ -14914,7 +14961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C251" s="12" t="s">
         <v>491</v>
       </c>
@@ -14951,7 +14998,7 @@
       <c r="T251" s="16">
         <v>2</v>
       </c>
-      <c r="U251" s="16">
+      <c r="U251" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V251" s="61">
@@ -14964,7 +15011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C252" s="12" t="s">
         <v>492</v>
       </c>
@@ -15001,7 +15048,7 @@
       <c r="T252" s="16">
         <v>2</v>
       </c>
-      <c r="U252" s="16">
+      <c r="U252" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V252" s="61">
@@ -15051,20 +15098,20 @@
       <c r="T253" s="16">
         <v>2</v>
       </c>
-      <c r="U253" s="16">
+      <c r="U253" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V253" s="61">
+        <v>0.03</v>
+      </c>
+      <c r="W253" s="61">
         <v>0</v>
-      </c>
-      <c r="W253" s="61">
-        <v>0.1</v>
       </c>
       <c r="X253" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="254" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C254" s="12" t="s">
         <v>494</v>
       </c>
@@ -15101,7 +15148,7 @@
       <c r="T254" s="16">
         <v>0</v>
       </c>
-      <c r="U254" s="16">
+      <c r="U254" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V254" s="61">
@@ -15114,7 +15161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C255" s="12" t="s">
         <v>496</v>
       </c>
@@ -15161,8 +15208,8 @@
       <c r="T255" s="16">
         <v>0</v>
       </c>
-      <c r="U255" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U255" s="67">
+        <v>0.1</v>
       </c>
       <c r="V255" s="61">
         <v>0.7</v>
@@ -15174,7 +15221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C256" s="12" t="s">
         <v>149</v>
       </c>
@@ -15205,11 +15252,11 @@
       <c r="R256" s="16"/>
       <c r="S256" s="16"/>
       <c r="T256" s="16"/>
-      <c r="U256" s="16"/>
+      <c r="U256" s="67"/>
       <c r="V256" s="61"/>
       <c r="W256" s="61"/>
     </row>
-    <row r="257" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C257" s="12" t="s">
         <v>499</v>
       </c>
@@ -15256,8 +15303,8 @@
       <c r="T257" s="16">
         <v>0</v>
       </c>
-      <c r="U257" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U257" s="67">
+        <v>0.1</v>
       </c>
       <c r="V257" s="61">
         <v>0.7</v>
@@ -15269,7 +15316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C258" s="12" t="s">
         <v>149</v>
       </c>
@@ -15300,11 +15347,11 @@
       <c r="R258" s="16"/>
       <c r="S258" s="16"/>
       <c r="T258" s="16"/>
-      <c r="U258" s="16"/>
+      <c r="U258" s="67"/>
       <c r="V258" s="61"/>
       <c r="W258" s="61"/>
     </row>
-    <row r="259" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C259" s="12" t="s">
         <v>501</v>
       </c>
@@ -15341,8 +15388,8 @@
       <c r="T259" s="16">
         <v>0</v>
       </c>
-      <c r="U259" s="16">
-        <v>0.41184999999999999</v>
+      <c r="U259" s="67">
+        <v>0.1</v>
       </c>
       <c r="V259" s="61">
         <v>0.4</v>
@@ -15354,7 +15401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C260" s="12" t="s">
         <v>503</v>
       </c>
@@ -15399,7 +15446,7 @@
       <c r="T260" s="16">
         <v>0</v>
       </c>
-      <c r="U260" s="16">
+      <c r="U260" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V260" s="61">
@@ -15412,7 +15459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C261" s="12" t="s">
         <v>504</v>
       </c>
@@ -15457,7 +15504,7 @@
       <c r="T261" s="16">
         <v>0</v>
       </c>
-      <c r="U261" s="16">
+      <c r="U261" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V261" s="61">
@@ -15470,7 +15517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C262" s="12" t="s">
         <v>505</v>
       </c>
@@ -15507,7 +15554,7 @@
       <c r="T262" s="16">
         <v>0</v>
       </c>
-      <c r="U262" s="16">
+      <c r="U262" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V262" s="61">
@@ -15520,7 +15567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C263" s="12" t="s">
         <v>507</v>
       </c>
@@ -15557,7 +15604,7 @@
       <c r="T263" s="16">
         <v>0</v>
       </c>
-      <c r="U263" s="16">
+      <c r="U263" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V263" s="61">
@@ -15570,7 +15617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C264" s="12" t="s">
         <v>509</v>
       </c>
@@ -15607,7 +15654,7 @@
       <c r="T264" s="16">
         <v>0</v>
       </c>
-      <c r="U264" s="16">
+      <c r="U264" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V264" s="61">
@@ -15620,7 +15667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C265" s="12" t="s">
         <v>511</v>
       </c>
@@ -15657,7 +15704,7 @@
       <c r="T265" s="16">
         <v>0</v>
       </c>
-      <c r="U265" s="16">
+      <c r="U265" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V265" s="61">
@@ -15670,7 +15717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C266" s="12" t="s">
         <v>513</v>
       </c>
@@ -15707,7 +15754,7 @@
       <c r="T266" s="16">
         <v>0</v>
       </c>
-      <c r="U266" s="16">
+      <c r="U266" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V266" s="61">
@@ -15720,7 +15767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C267" s="12" t="s">
         <v>515</v>
       </c>
@@ -15757,7 +15804,7 @@
       <c r="T267" s="16">
         <v>0</v>
       </c>
-      <c r="U267" s="16">
+      <c r="U267" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V267" s="61">
@@ -15770,7 +15817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C268" s="12" t="s">
         <v>517</v>
       </c>
@@ -15807,7 +15854,7 @@
       <c r="T268" s="16">
         <v>7</v>
       </c>
-      <c r="U268" s="16">
+      <c r="U268" s="67">
         <v>0.1</v>
       </c>
       <c r="V268" s="61">
@@ -15820,7 +15867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C269" s="12" t="s">
         <v>520</v>
       </c>
@@ -15857,7 +15904,7 @@
       <c r="T269" s="16">
         <v>7</v>
       </c>
-      <c r="U269" s="16">
+      <c r="U269" s="67">
         <v>0.1</v>
       </c>
       <c r="V269" s="61">
@@ -15870,7 +15917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C270" s="12" t="s">
         <v>522</v>
       </c>
@@ -15907,13 +15954,13 @@
       <c r="T270" s="16">
         <v>7</v>
       </c>
-      <c r="U270" s="16">
+      <c r="U270" s="67">
         <v>0.1</v>
       </c>
       <c r="V270" s="61"/>
       <c r="W270" s="61"/>
     </row>
-    <row r="271" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C271" s="12" t="s">
         <v>524</v>
       </c>
@@ -15950,13 +15997,13 @@
       <c r="T271" s="16">
         <v>5</v>
       </c>
-      <c r="U271" s="16">
+      <c r="U271" s="67">
         <v>0.1</v>
       </c>
       <c r="V271" s="61"/>
       <c r="W271" s="61"/>
     </row>
-    <row r="272" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="C272" s="12" t="s">
         <v>526</v>
       </c>
@@ -15993,7 +16040,7 @@
       <c r="T272" s="16">
         <v>0</v>
       </c>
-      <c r="U272" s="16">
+      <c r="U272" s="67">
         <v>0.1</v>
       </c>
       <c r="V272" s="61"/>
@@ -16044,13 +16091,13 @@
       <c r="T273" s="16">
         <v>2</v>
       </c>
-      <c r="U273" s="16">
+      <c r="U273" s="67">
         <v>0.1</v>
       </c>
       <c r="V273" s="61"/>
       <c r="W273" s="61"/>
     </row>
-    <row r="274" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C274" s="12" t="s">
         <v>530</v>
       </c>
@@ -16087,13 +16134,13 @@
       <c r="T274" s="16">
         <v>5</v>
       </c>
-      <c r="U274" s="16">
+      <c r="U274" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V274" s="61"/>
       <c r="W274" s="61"/>
     </row>
-    <row r="275" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C275" s="12" t="s">
         <v>533</v>
       </c>
@@ -16130,13 +16177,13 @@
       <c r="T275" s="16">
         <v>5</v>
       </c>
-      <c r="U275" s="16">
+      <c r="U275" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V275" s="61"/>
       <c r="W275" s="61"/>
     </row>
-    <row r="276" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C276" s="12" t="s">
         <v>535</v>
       </c>
@@ -16173,13 +16220,13 @@
       <c r="T276" s="16">
         <v>5</v>
       </c>
-      <c r="U276" s="16">
+      <c r="U276" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V276" s="61"/>
       <c r="W276" s="61"/>
     </row>
-    <row r="277" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C277" s="12" t="s">
         <v>537</v>
       </c>
@@ -16220,7 +16267,7 @@
       <c r="T277" s="16">
         <v>0</v>
       </c>
-      <c r="U277" s="16">
+      <c r="U277" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V277" s="60"/>
@@ -16271,13 +16318,13 @@
       <c r="T278" s="16">
         <v>2</v>
       </c>
-      <c r="U278" s="16">
+      <c r="U278" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V278" s="60"/>
       <c r="W278" s="60"/>
     </row>
-    <row r="279" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C279" s="12" t="s">
         <v>149</v>
       </c>
@@ -16314,13 +16361,13 @@
       <c r="T279" s="16">
         <v>5</v>
       </c>
-      <c r="U279" s="16">
+      <c r="U279" s="67">
         <v>0.54913299999999998</v>
       </c>
       <c r="V279" s="60"/>
       <c r="W279" s="60"/>
     </row>
-    <row r="280" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C280" s="12" t="s">
         <v>556</v>
       </c>
@@ -16365,13 +16412,13 @@
       <c r="T280" s="16">
         <v>0</v>
       </c>
-      <c r="U280" s="16">
+      <c r="U280" s="67">
         <v>0.27456599999999998</v>
       </c>
       <c r="V280" s="60"/>
       <c r="W280" s="60"/>
     </row>
-    <row r="281" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="C281" s="12" t="s">
         <v>557</v>
       </c>
@@ -16416,7 +16463,7 @@
       <c r="T281" s="16">
         <v>0</v>
       </c>
-      <c r="U281" s="16">
+      <c r="U281" s="67">
         <v>0.108447</v>
       </c>
       <c r="V281" s="60"/>
@@ -16441,7 +16488,7 @@
       <c r="R282" s="16"/>
       <c r="S282" s="16"/>
       <c r="T282" s="16"/>
-      <c r="U282" s="16"/>
+      <c r="U282" s="67"/>
       <c r="V282" s="61"/>
       <c r="W282" s="61"/>
     </row>
@@ -16464,7 +16511,7 @@
       <c r="R283" s="16"/>
       <c r="S283" s="16"/>
       <c r="T283" s="16"/>
-      <c r="U283" s="16"/>
+      <c r="U283" s="67"/>
     </row>
     <row r="284" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C284" s="17" t="s">
@@ -25650,16 +25697,22 @@
       <c r="G1204" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="C3:X281"/>
+  <autoFilter ref="C3:X281" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="COMH2R"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:W118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>